<commit_message>
ola electric content push
</commit_message>
<xml_diff>
--- a/ola_electric/stats_prob/Stats Data Examples.xlsx
+++ b/ola_electric/stats_prob/Stats Data Examples.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunnvant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/Work/Vired/Content/corp_trainings/ola_electric/stats_prob/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_F64FE6B39587F65BA08A61299A01FF5137E9FD09" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{640B55B9-2DBF-6F4F-A5D0-B3FFD5797AC9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="15" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binomial" sheetId="1" r:id="rId1"/>
@@ -18,23 +19,24 @@
     <sheet name="ANOVA Layout Test" sheetId="4" r:id="rId4"/>
     <sheet name="Chi Square " sheetId="5" r:id="rId5"/>
     <sheet name="Cricket" sheetId="6" r:id="rId6"/>
-    <sheet name="Two Sample" sheetId="7" r:id="rId7"/>
-    <sheet name="Single Factor" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet3" sheetId="21" r:id="rId9"/>
-    <sheet name="SSW" sheetId="9" r:id="rId10"/>
-    <sheet name="SSB " sheetId="10" r:id="rId11"/>
-    <sheet name="Two Factor" sheetId="11" r:id="rId12"/>
-    <sheet name="Angel of Death" sheetId="17" r:id="rId13"/>
-    <sheet name="Coke and Pespsi" sheetId="12" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="18" r:id="rId15"/>
-    <sheet name="Loaded Dice" sheetId="13" r:id="rId16"/>
-    <sheet name="Post hoc" sheetId="14" r:id="rId17"/>
-    <sheet name="Studentised t" sheetId="15" r:id="rId18"/>
-    <sheet name="Categorical Association" sheetId="19" r:id="rId19"/>
-    <sheet name="Simple Hypothesis Tests" sheetId="22" r:id="rId20"/>
+    <sheet name="Sheet2" sheetId="23" r:id="rId7"/>
+    <sheet name="Two Sample" sheetId="7" r:id="rId8"/>
+    <sheet name="Single Factor" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="21" r:id="rId10"/>
+    <sheet name="SSW" sheetId="9" r:id="rId11"/>
+    <sheet name="SSB " sheetId="10" r:id="rId12"/>
+    <sheet name="Two Factor" sheetId="11" r:id="rId13"/>
+    <sheet name="Angel of Death" sheetId="17" r:id="rId14"/>
+    <sheet name="Coke and Pespsi" sheetId="12" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId16"/>
+    <sheet name="Loaded Dice" sheetId="13" r:id="rId17"/>
+    <sheet name="Post hoc" sheetId="14" r:id="rId18"/>
+    <sheet name="Studentised t" sheetId="15" r:id="rId19"/>
+    <sheet name="Categorical Association" sheetId="19" r:id="rId20"/>
+    <sheet name="Simple Hypothesis Tests" sheetId="22" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
     <definedName name="n_1">'[1]t-test'!$B$13</definedName>
@@ -51,17 +53,27 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="154">
   <si>
     <t>SHIPPING_CITY</t>
   </si>
@@ -520,11 +532,56 @@
   <si>
     <t>If population conditional distribution for one variable is same for all the categories of the other variable</t>
   </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Equal Variances</t>
+  </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Pooled Variance</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -960,7 +1017,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1183,11 +1240,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1205,7 +1263,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1411,7 +1469,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1448,7 +1512,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1495,7 +1565,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1547,7 +1623,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1607,7 +1689,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1645,7 +1733,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1697,7 +1791,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1749,7 +1849,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Oval 4"/>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1908,7 +2014,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2291,7 +2403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
@@ -2300,19 +2412,19 @@
       <selection pane="bottomLeft" activeCell="C23" sqref="C23:G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" style="3"/>
+    <col min="21" max="21" width="8.6640625" style="3"/>
     <col min="22" max="22" width="10" style="3" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2342,7 +2454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -2376,7 +2488,7 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2410,7 +2522,7 @@
         <v>0.41025641025641024</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2444,7 +2556,7 @@
         <v>1.5384615384615385</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2478,7 +2590,7 @@
         <v>0.92307692307692313</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2512,7 +2624,7 @@
         <v>0.53846153846153855</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2546,7 +2658,7 @@
         <v>1.0256410256410255</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2580,7 +2692,7 @@
         <v>0.92307692307692302</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -2614,7 +2726,7 @@
         <v>0.25641025641025639</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2648,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2682,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2716,7 +2828,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2743,7 +2855,7 @@
         <v>6.1794871794871797</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -2760,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2777,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -2788,7 +2900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -2799,7 +2911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -2810,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -2821,7 +2933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -2832,7 +2944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -2850,7 +2962,7 @@
         <v>0.35897435897435898</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -2861,7 +2973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -2879,7 +2991,7 @@
         <v>0.16844844849503837</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -2890,7 +3002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>11</v>
       </c>
@@ -2905,7 +3017,7 @@
         <v>0.83141554359722303</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -2916,7 +3028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -2927,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2938,7 +3050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -2949,7 +3061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -2960,7 +3072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -2971,7 +3083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
@@ -2982,7 +3094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -2993,7 +3105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>11</v>
       </c>
@@ -3004,7 +3116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -3015,7 +3127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>10</v>
       </c>
@@ -3026,7 +3138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
@@ -3037,7 +3149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -3048,7 +3160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>11</v>
       </c>
@@ -3070,7 +3182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>17</v>
       </c>
@@ -3087,7 +3199,7 @@
         <v>0.8974358974358978</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D42" s="3">
         <f>D41/C41</f>
         <v>0.16990291262135929</v>
@@ -3101,20 +3213,32 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="2" customWidth="1"/>
-    <col min="12" max="12" width="1.140625" customWidth="1"/>
+    <col min="12" max="12" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
         <v>64</v>
       </c>
@@ -3125,7 +3249,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>58</v>
       </c>
@@ -3172,7 +3296,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="50">
         <v>210.5</v>
       </c>
@@ -3229,7 +3353,7 @@
         <v>95.648400000000024</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="50">
         <v>198.1</v>
       </c>
@@ -3286,7 +3410,7 @@
         <v>1.0404000000000209</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="50">
         <v>145.30000000000001</v>
       </c>
@@ -3343,7 +3467,7 @@
         <v>4.9283999999999946</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="50">
         <v>185.5</v>
       </c>
@@ -3400,7 +3524,7 @@
         <v>429.31839999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="50">
         <v>189.1</v>
       </c>
@@ -3457,7 +3581,7 @@
         <v>17.808399999999992</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="50">
         <v>135.9</v>
       </c>
@@ -3514,7 +3638,7 @@
         <v>8.8803999999999395</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="50">
         <v>180</v>
       </c>
@@ -3571,7 +3695,7 @@
         <v>6.350400000000052</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="50">
         <v>149.4</v>
       </c>
@@ -3628,7 +3752,7 @@
         <v>0.67239999999998878</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="50">
         <v>176.4</v>
       </c>
@@ -3685,7 +3809,7 @@
         <v>107.7443999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="50">
         <v>229</v>
       </c>
@@ -3742,7 +3866,7 @@
         <v>70.224399999999918</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <f>AVERAGE(A3:A12)</f>
         <v>179.92000000000002</v>
@@ -3764,7 +3888,7 @@
         <v>178.72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>67</v>
       </c>
@@ -3776,7 +3900,7 @@
         <v>34735.021999999983</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E16">
         <f>E14/45</f>
         <v>771.88937777777744</v>
@@ -3787,26 +3911,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
@@ -3823,7 +3947,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="50">
         <v>210.5</v>
       </c>
@@ -3840,7 +3964,7 @@
         <v>188.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="50">
         <v>198.1</v>
       </c>
@@ -3857,7 +3981,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="50">
         <v>145.30000000000001</v>
       </c>
@@ -3874,7 +3998,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="50">
         <v>185.5</v>
       </c>
@@ -3891,7 +4015,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="50">
         <v>189.1</v>
       </c>
@@ -3908,7 +4032,7 @@
         <v>174.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="50">
         <v>135.9</v>
       </c>
@@ -3925,7 +4049,7 @@
         <v>181.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="50">
         <v>180</v>
       </c>
@@ -3942,7 +4066,7 @@
         <v>176.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="50">
         <v>149.4</v>
       </c>
@@ -3959,7 +4083,7 @@
         <v>177.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="50">
         <v>176.4</v>
       </c>
@@ -3976,7 +4100,7 @@
         <v>189.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="50">
         <v>229</v>
       </c>
@@ -3993,7 +4117,7 @@
         <v>187.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="52">
         <f>AVERAGE(B3:B12)</f>
         <v>179.92000000000002</v>
@@ -4015,7 +4139,7 @@
         <v>178.72</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="54" t="s">
         <v>68</v>
       </c>
@@ -4028,7 +4152,7 @@
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="54" t="s">
         <v>69</v>
       </c>
@@ -4053,7 +4177,7 @@
         <v>7.9523999999999617</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
         <v>70</v>
       </c>
@@ -4078,7 +4202,7 @@
         <v>79.523999999999617</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
         <v>71</v>
       </c>
@@ -4090,344 +4214,6 @@
       <c r="D17" s="54"/>
       <c r="E17" s="54"/>
       <c r="F17" s="54"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="56">
-        <v>1</v>
-      </c>
-      <c r="B2" s="56">
-        <v>1</v>
-      </c>
-      <c r="C2" s="56">
-        <v>106.9</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="56">
-        <v>106.9</v>
-      </c>
-      <c r="G2" s="56">
-        <v>100.2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
-        <v>1</v>
-      </c>
-      <c r="B3" s="56">
-        <v>1</v>
-      </c>
-      <c r="C3" s="56">
-        <v>84</v>
-      </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56">
-        <v>84</v>
-      </c>
-      <c r="G3" s="56">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="56">
-        <v>1</v>
-      </c>
-      <c r="B4" s="56">
-        <v>1</v>
-      </c>
-      <c r="C4" s="56">
-        <v>97.5</v>
-      </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56">
-        <v>97.5</v>
-      </c>
-      <c r="G4" s="56">
-        <v>118.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
-        <v>1</v>
-      </c>
-      <c r="B5" s="56">
-        <v>1</v>
-      </c>
-      <c r="C5" s="56">
-        <v>97.1</v>
-      </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56">
-        <v>97.1</v>
-      </c>
-      <c r="G5" s="56">
-        <v>104.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
-        <v>1</v>
-      </c>
-      <c r="B6" s="56">
-        <v>1</v>
-      </c>
-      <c r="C6" s="56">
-        <v>99.5</v>
-      </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56">
-        <v>99.5</v>
-      </c>
-      <c r="G6" s="56">
-        <v>111.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="56">
-        <v>1</v>
-      </c>
-      <c r="B7" s="56">
-        <v>2</v>
-      </c>
-      <c r="C7" s="56">
-        <v>100.2</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="56">
-        <v>82.8</v>
-      </c>
-      <c r="G7" s="56">
-        <v>89.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="56">
-        <v>1</v>
-      </c>
-      <c r="B8" s="56">
-        <v>2</v>
-      </c>
-      <c r="C8" s="56">
-        <v>101</v>
-      </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56">
-        <v>80.400000000000006</v>
-      </c>
-      <c r="G8" s="56">
-        <v>106.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
-        <v>1</v>
-      </c>
-      <c r="B9" s="56">
-        <v>2</v>
-      </c>
-      <c r="C9" s="56">
-        <v>118.5</v>
-      </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56">
-        <v>95.6</v>
-      </c>
-      <c r="G9" s="56">
-        <v>98.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="56">
-        <v>1</v>
-      </c>
-      <c r="B10" s="56">
-        <v>2</v>
-      </c>
-      <c r="C10" s="56">
-        <v>104.5</v>
-      </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56">
-        <v>82</v>
-      </c>
-      <c r="G10" s="56">
-        <v>89.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="56">
-        <v>1</v>
-      </c>
-      <c r="B11" s="56">
-        <v>2</v>
-      </c>
-      <c r="C11" s="56">
-        <v>111.2</v>
-      </c>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56">
-        <v>83.2</v>
-      </c>
-      <c r="G11" s="56">
-        <v>104.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="56">
-        <v>2</v>
-      </c>
-      <c r="B12" s="56">
-        <v>1</v>
-      </c>
-      <c r="C12" s="56">
-        <v>82.8</v>
-      </c>
-      <c r="E12" s="56"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
-        <v>2</v>
-      </c>
-      <c r="B13" s="56">
-        <v>1</v>
-      </c>
-      <c r="C13" s="56">
-        <v>80.400000000000006</v>
-      </c>
-      <c r="E13" s="56"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="56">
-        <v>2</v>
-      </c>
-      <c r="B14" s="56">
-        <v>1</v>
-      </c>
-      <c r="C14" s="56">
-        <v>95.6</v>
-      </c>
-      <c r="E14" s="56"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="56">
-        <v>2</v>
-      </c>
-      <c r="B15" s="56">
-        <v>1</v>
-      </c>
-      <c r="C15" s="56">
-        <v>82</v>
-      </c>
-      <c r="E15" s="56"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="56">
-        <v>2</v>
-      </c>
-      <c r="B16" s="56">
-        <v>1</v>
-      </c>
-      <c r="C16" s="56">
-        <v>83.2</v>
-      </c>
-      <c r="E16" s="56"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="56">
-        <v>2</v>
-      </c>
-      <c r="B17" s="56">
-        <v>2</v>
-      </c>
-      <c r="C17" s="56">
-        <v>89.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
-        <v>2</v>
-      </c>
-      <c r="B18" s="56">
-        <v>2</v>
-      </c>
-      <c r="C18" s="56">
-        <v>106.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="56">
-        <v>2</v>
-      </c>
-      <c r="B19" s="56">
-        <v>2</v>
-      </c>
-      <c r="C19" s="56">
-        <v>98.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="56">
-        <v>2</v>
-      </c>
-      <c r="B20" s="56">
-        <v>2</v>
-      </c>
-      <c r="C20" s="56">
-        <v>89.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
-        <v>2</v>
-      </c>
-      <c r="B21" s="56">
-        <v>2</v>
-      </c>
-      <c r="C21" s="56">
-        <v>104.6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4435,21 +4221,362 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="225" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="56">
+        <v>1</v>
+      </c>
+      <c r="B2" s="56">
+        <v>1</v>
+      </c>
+      <c r="C2" s="56">
+        <v>106.9</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="56">
+        <v>106.9</v>
+      </c>
+      <c r="G2" s="56">
+        <v>100.2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="56">
+        <v>1</v>
+      </c>
+      <c r="B3" s="56">
+        <v>1</v>
+      </c>
+      <c r="C3" s="56">
+        <v>84</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56">
+        <v>84</v>
+      </c>
+      <c r="G3" s="56">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="56">
+        <v>1</v>
+      </c>
+      <c r="B4" s="56">
+        <v>1</v>
+      </c>
+      <c r="C4" s="56">
+        <v>97.5</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56">
+        <v>97.5</v>
+      </c>
+      <c r="G4" s="56">
+        <v>118.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="56">
+        <v>1</v>
+      </c>
+      <c r="B5" s="56">
+        <v>1</v>
+      </c>
+      <c r="C5" s="56">
+        <v>97.1</v>
+      </c>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56">
+        <v>97.1</v>
+      </c>
+      <c r="G5" s="56">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="56">
+        <v>1</v>
+      </c>
+      <c r="B6" s="56">
+        <v>1</v>
+      </c>
+      <c r="C6" s="56">
+        <v>99.5</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56">
+        <v>99.5</v>
+      </c>
+      <c r="G6" s="56">
+        <v>111.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="56">
+        <v>1</v>
+      </c>
+      <c r="B7" s="56">
+        <v>2</v>
+      </c>
+      <c r="C7" s="56">
+        <v>100.2</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="56">
+        <v>82.8</v>
+      </c>
+      <c r="G7" s="56">
+        <v>89.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="56">
+        <v>1</v>
+      </c>
+      <c r="B8" s="56">
+        <v>2</v>
+      </c>
+      <c r="C8" s="56">
+        <v>101</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="G8" s="56">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="56">
+        <v>1</v>
+      </c>
+      <c r="B9" s="56">
+        <v>2</v>
+      </c>
+      <c r="C9" s="56">
+        <v>118.5</v>
+      </c>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56">
+        <v>95.6</v>
+      </c>
+      <c r="G9" s="56">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="56">
+        <v>1</v>
+      </c>
+      <c r="B10" s="56">
+        <v>2</v>
+      </c>
+      <c r="C10" s="56">
+        <v>104.5</v>
+      </c>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56">
+        <v>82</v>
+      </c>
+      <c r="G10" s="56">
+        <v>89.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="56">
+        <v>1</v>
+      </c>
+      <c r="B11" s="56">
+        <v>2</v>
+      </c>
+      <c r="C11" s="56">
+        <v>111.2</v>
+      </c>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56">
+        <v>83.2</v>
+      </c>
+      <c r="G11" s="56">
+        <v>104.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="56">
+        <v>2</v>
+      </c>
+      <c r="B12" s="56">
+        <v>1</v>
+      </c>
+      <c r="C12" s="56">
+        <v>82.8</v>
+      </c>
+      <c r="E12" s="56"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="56">
+        <v>2</v>
+      </c>
+      <c r="B13" s="56">
+        <v>1</v>
+      </c>
+      <c r="C13" s="56">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="E13" s="56"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="56">
+        <v>2</v>
+      </c>
+      <c r="B14" s="56">
+        <v>1</v>
+      </c>
+      <c r="C14" s="56">
+        <v>95.6</v>
+      </c>
+      <c r="E14" s="56"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="56">
+        <v>2</v>
+      </c>
+      <c r="B15" s="56">
+        <v>1</v>
+      </c>
+      <c r="C15" s="56">
+        <v>82</v>
+      </c>
+      <c r="E15" s="56"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="56">
+        <v>2</v>
+      </c>
+      <c r="B16" s="56">
+        <v>1</v>
+      </c>
+      <c r="C16" s="56">
+        <v>83.2</v>
+      </c>
+      <c r="E16" s="56"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="56">
+        <v>2</v>
+      </c>
+      <c r="B17" s="56">
+        <v>2</v>
+      </c>
+      <c r="C17" s="56">
+        <v>89.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="56">
+        <v>2</v>
+      </c>
+      <c r="B18" s="56">
+        <v>2</v>
+      </c>
+      <c r="C18" s="56">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="56">
+        <v>2</v>
+      </c>
+      <c r="B19" s="56">
+        <v>2</v>
+      </c>
+      <c r="C19" s="56">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="56">
+        <v>2</v>
+      </c>
+      <c r="B20" s="56">
+        <v>2</v>
+      </c>
+      <c r="C20" s="56">
+        <v>89.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="56">
+        <v>2</v>
+      </c>
+      <c r="B21" s="56">
+        <v>2</v>
+      </c>
+      <c r="C21" s="56">
+        <v>104.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>111</v>
       </c>
@@ -4457,12 +4584,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="80" t="s">
         <v>106</v>
       </c>
@@ -4472,7 +4599,7 @@
       <c r="C3" s="83"/>
       <c r="D3" s="84"/>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="81"/>
       <c r="B4" s="73" t="s">
         <v>108</v>
@@ -4484,7 +4611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="73" t="s">
         <v>108</v>
       </c>
@@ -4498,7 +4625,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="73" t="s">
         <v>109</v>
       </c>
@@ -4512,7 +4639,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="73" t="s">
         <v>56</v>
       </c>
@@ -4526,12 +4653,12 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="80" t="s">
         <v>106</v>
       </c>
@@ -4541,7 +4668,7 @@
       <c r="C11" s="83"/>
       <c r="D11" s="84"/>
     </row>
-    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="81"/>
       <c r="B12" s="73" t="s">
         <v>108</v>
@@ -4553,29 +4680,47 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
+      <c r="B13" s="75">
+        <f>D5*B7/D7</f>
+        <v>11.589274832419257</v>
+      </c>
+      <c r="C13" s="75">
+        <f>D5*C7/D7</f>
+        <v>245.41072516758075</v>
+      </c>
       <c r="D13" s="76"/>
     </row>
-    <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
+      <c r="B14" s="75">
+        <f>D6*B7/D7</f>
+        <v>62.410725167580743</v>
+      </c>
+      <c r="C14" s="75">
+        <f>D6*C7/D7</f>
+        <v>1321.5892748324193</v>
+      </c>
       <c r="D14" s="76"/>
     </row>
-    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="73" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="75"/>
       <c r="C15" s="75"/>
       <c r="D15" s="76"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>_xlfn.CHISQ.TEST(B5:C6,B13:C14)</f>
+        <v>1.4108986534997488E-20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4588,17 +4733,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -4606,7 +4751,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
         <v>79</v>
       </c>
@@ -4638,7 +4783,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -4663,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -4688,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -4713,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -4758,34 +4903,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>86</v>
       </c>
@@ -4794,7 +4939,7 @@
       </c>
       <c r="C1" s="58"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4802,7 +4947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4810,7 +4955,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4818,7 +4963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4831,23 +4976,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="59" t="s">
         <v>114</v>
       </c>
@@ -4862,7 +5007,7 @@
       </c>
       <c r="F1" s="60"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="61">
         <v>78</v>
       </c>
@@ -4877,7 +5022,7 @@
       </c>
       <c r="F2" s="62"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="63">
         <v>87</v>
       </c>
@@ -4892,7 +5037,7 @@
       </c>
       <c r="F3" s="62"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64">
         <v>81</v>
       </c>
@@ -4907,7 +5052,7 @@
       </c>
       <c r="F4" s="62"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="63">
         <v>89</v>
       </c>
@@ -4922,7 +5067,7 @@
       </c>
       <c r="F5" s="62"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="64">
         <v>85</v>
       </c>
@@ -4937,7 +5082,7 @@
       </c>
       <c r="F6" s="62"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -4959,11 +5104,11 @@
       </c>
       <c r="F7" s="66"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E8" s="67"/>
       <c r="F8" s="68"/>
     </row>
-    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="D9" s="69"/>
       <c r="E9" s="70"/>
       <c r="F9" s="70"/>
@@ -4971,7 +5116,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="71" t="s">
         <v>90</v>
       </c>
@@ -4995,7 +5140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="72" t="s">
         <v>96</v>
       </c>
@@ -5013,7 +5158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="72" t="s">
         <v>99</v>
       </c>
@@ -5027,7 +5172,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="72" t="s">
         <v>101</v>
       </c>
@@ -5043,7 +5188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="72" t="s">
         <v>103</v>
       </c>
@@ -5052,7 +5197,7 @@
       <c r="E14" s="72"/>
       <c r="F14" s="68"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="72" t="s">
         <v>104</v>
       </c>
@@ -5061,7 +5206,7 @@
       <c r="E15" s="72"/>
       <c r="F15" s="68"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="72" t="s">
         <v>105</v>
       </c>
@@ -5076,44 +5221,443 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>405</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>406</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>407</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>408</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>409</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>410</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>411</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>412</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>413</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>414</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>415</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>416</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>417</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>418</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>419</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>420</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>421</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>422</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>423</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>424</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>425</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>426</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>427</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>428</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>429</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>430</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>431</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>432</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>433</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>434</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>435</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>436</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="21"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>437</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="21"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>438</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="21"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>439</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="21"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>440</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="21"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>441</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>442</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="21"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>443</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="21"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>444</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="21"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>445</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="21"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>446</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="21"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>447</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="21"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>448</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="21"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>449</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="21"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>450</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A2:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView topLeftCell="I1" zoomScale="235" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C2" s="85" t="s">
         <v>127</v>
       </c>
@@ -5127,7 +5671,7 @@
       </c>
       <c r="R2" s="85"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
         <v>120</v>
       </c>
@@ -5174,7 +5718,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="77" t="s">
         <v>121</v>
       </c>
@@ -5227,7 +5771,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="77" t="s">
         <v>122</v>
       </c>
@@ -5280,7 +5824,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="77" t="s">
         <v>123</v>
       </c>
@@ -5319,24 +5863,15 @@
       <c r="O6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="P6" s="77">
-        <f>SUM(P4:P5)</f>
-        <v>959</v>
-      </c>
-      <c r="Q6" s="77">
-        <f t="shared" ref="Q6" si="1">SUM(Q4:Q5)</f>
-        <v>991</v>
-      </c>
-      <c r="R6" s="77">
-        <f>SUM(R4:R5)</f>
-        <v>821</v>
-      </c>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
       <c r="S6" s="77">
-        <f t="shared" ref="S6" si="2">SUM(S4:S5)</f>
+        <f t="shared" ref="S6" si="1">SUM(S4:S5)</f>
         <v>2771</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="77" t="s">
         <v>56</v>
       </c>
@@ -5345,19 +5880,19 @@
         <v>594</v>
       </c>
       <c r="C7" s="77">
-        <f t="shared" ref="C7:E7" si="3">SUM(C4:C6)</f>
+        <f t="shared" ref="C7:E7" si="2">SUM(C4:C6)</f>
         <v>189</v>
       </c>
       <c r="D7" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>567</v>
       </c>
       <c r="E7" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1350</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C9" s="85" t="s">
         <v>127</v>
       </c>
@@ -5370,7 +5905,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
         <v>120</v>
       </c>
@@ -5417,7 +5952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="77" t="s">
         <v>121</v>
       </c>
@@ -5459,7 +5994,7 @@
       </c>
       <c r="P11" s="77">
         <f>(I4-P4)/SQRT(P4*(1-S4/S6)*(1-P6/S6))</f>
-        <v>4.0150898278951912</v>
+        <v>3.2468042052201231</v>
       </c>
       <c r="Q11" s="77">
         <v>516</v>
@@ -5471,7 +6006,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="77" t="s">
         <v>122</v>
       </c>
@@ -5513,7 +6048,7 @@
       </c>
       <c r="P12" s="77">
         <f>(I5-P5)/SQRT(P5*(1-S5/S6)*(1-P6/S6))</f>
-        <v>-4.0150898278951956</v>
+        <v>-3.2468042052201271</v>
       </c>
       <c r="Q12" s="77">
         <v>475</v>
@@ -5525,7 +6060,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="77" t="s">
         <v>123</v>
       </c>
@@ -5576,7 +6111,7 @@
         <v>2771</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="78" t="s">
         <v>128</v>
       </c>
@@ -5584,15 +6119,19 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="78" t="s">
         <v>129</v>
       </c>
       <c r="H16" s="78" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O16" s="21">
+        <f>_xlfn.CHISQ.TEST(I4:K5,P4:R5)</f>
+        <v>3.0327729089393412E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C19" s="85" t="s">
         <v>127</v>
       </c>
@@ -5602,7 +6141,7 @@
       </c>
       <c r="K19" s="85"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="58" t="s">
         <v>120</v>
       </c>
@@ -5634,7 +6173,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="77" t="s">
         <v>121</v>
       </c>
@@ -5672,7 +6211,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="77" t="s">
         <v>122</v>
       </c>
@@ -5710,7 +6249,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="77" t="s">
         <v>123</v>
       </c>
@@ -5745,7 +6284,7 @@
         <v>2771</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="77" t="s">
         <v>56</v>
       </c>
@@ -5762,27 +6301,27 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="78" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="78" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>138</v>
       </c>
@@ -5802,435 +6341,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>405</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>406</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>407</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>408</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>409</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>410</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>411</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>412</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>413</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>414</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>415</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>416</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>417</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>418</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>419</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>420</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>421</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>422</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>423</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>424</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>425</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>426</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>427</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>428</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="21"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>429</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>430</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>431</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>432</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>433</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>434</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>435</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>436</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="21"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>437</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>438</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>439</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>440</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>441</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>442</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>443</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="21"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>444</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="21"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>445</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>446</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>447</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>448</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>449</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>450</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="185" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:G31"/>
+    <sheetView zoomScale="244" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
@@ -6247,7 +6387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -6264,7 +6404,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -6281,7 +6421,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -6298,7 +6438,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -6315,7 +6455,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -6332,7 +6472,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -6349,7 +6489,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -6366,7 +6506,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -6383,7 +6523,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -6402,7 +6542,7 @@
         <v>158.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -6413,7 +6553,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -6432,19 +6572,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="26" t="s">
         <v>25</v>
       </c>
@@ -6458,7 +6598,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="27">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -6472,7 +6612,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="27">
         <v>2.4E-2</v>
       </c>
@@ -6486,7 +6626,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="27">
         <v>2.1000000000000001E-2</v>
       </c>
@@ -6500,7 +6640,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="27">
         <v>2.7E-2</v>
       </c>
@@ -6514,7 +6654,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="27">
         <v>2.2499999999999999E-2</v>
       </c>
@@ -6528,7 +6668,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="27">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -6542,7 +6682,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>29</v>
       </c>
@@ -6563,44 +6703,44 @@
         <v>2.5166666666666667E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -6609,7 +6749,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -6618,7 +6758,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -6627,7 +6767,7 @@
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -6636,7 +6776,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -6652,23 +6792,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="32" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="32" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="32" customWidth="1"/>
+    <col min="4" max="4" width="2.5" style="32" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="32" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="32" customWidth="1"/>
     <col min="7" max="7" width="14" style="32" customWidth="1"/>
-    <col min="8" max="16384" width="29.5703125" style="32"/>
+    <col min="8" max="16384" width="29.5" style="32"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -6763,24 +6903,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="290" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="3"/>
+    <col min="2" max="4" width="9.1640625" style="3"/>
     <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="9" width="9.1640625" style="3"/>
+    <col min="10" max="10" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -6791,7 +6931,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
@@ -6805,7 +6945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -6833,7 +6973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -6861,7 +7001,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="38">
         <f>B3+B4</f>
         <v>234</v>
@@ -6887,7 +7027,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -6896,7 +7036,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -6908,26 +7048,45 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <f>D3*B5/D5</f>
+        <v>25.341013824884794</v>
+      </c>
+      <c r="C9" s="3">
+        <f>D3*C5/D5</f>
+        <v>21.658986175115206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B10" s="3">
+        <f>D4*B5/D5</f>
+        <v>208.65898617511522</v>
+      </c>
+      <c r="C10" s="3">
+        <f>D4*C5/D5</f>
+        <v>178.34101382488478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="41">
+        <f>_xlfn.CHISQ.TEST(B3:C4,B9:C10)</f>
+        <v>1.7623181857197887E-2</v>
+      </c>
       <c r="G12" s="41"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -6940,7 +7099,7 @@
         <v>0.76470588235294112</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D16" s="3">
         <f>B4/D4</f>
         <v>0.51937984496124034</v>
@@ -6950,7 +7109,7 @@
         <v>0.65986394557823125</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="42" t="s">
         <v>45</v>
       </c>
@@ -6960,7 +7119,7 @@
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="43" t="s">
         <v>46</v>
       </c>
@@ -6970,7 +7129,7 @@
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="44"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -6978,7 +7137,7 @@
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:10" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45" t="s">
         <v>47</v>
       </c>
@@ -6996,7 +7155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>52</v>
       </c>
@@ -7020,7 +7179,7 @@
         <v>57.870370370370374</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
         <v>53</v>
       </c>
@@ -7041,7 +7200,7 @@
         <v>34.722222222222229</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
         <v>54</v>
       </c>
@@ -7062,7 +7221,7 @@
         <v>6.9444444444444473</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45" t="s">
         <v>55</v>
       </c>
@@ -7083,7 +7242,7 @@
         <v>0.46296296296296285</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
         <v>56</v>
       </c>
@@ -7104,24 +7263,163 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11F253C-B485-2549-B370-D8B014EF6528}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView zoomScale="222" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12">
+        <v>8.75</v>
+      </c>
+      <c r="C4" s="12">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="12">
+        <v>4.6805555555555554</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5.8444444444444468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="12">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="12">
+        <v>5.2625000000000011</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="12">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1.4133735186028802</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="12">
+        <v>8.73032878010674E-2</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1.7340636066175394</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="86">
+        <v>0.1746065756021348</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="15">
+        <v>2.1009220402410378</v>
+      </c>
+      <c r="C14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="G3:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="B1" zoomScale="224" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G3" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="7:17" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G4" s="3">
         <v>8.5</v>
       </c>
@@ -7129,7 +7427,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G5" s="3">
         <v>9.5</v>
       </c>
@@ -7143,7 +7441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G6" s="3">
         <v>10</v>
       </c>
@@ -7157,7 +7455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G7" s="3">
         <v>7</v>
       </c>
@@ -7171,7 +7469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G8" s="3">
         <v>12.5</v>
       </c>
@@ -7185,7 +7483,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G9" s="3">
         <v>9</v>
       </c>
@@ -7199,7 +7497,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G10" s="3">
         <v>4</v>
       </c>
@@ -7213,7 +7511,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G11" s="3">
         <v>9</v>
       </c>
@@ -7227,7 +7525,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G12" s="3">
         <v>9</v>
       </c>
@@ -7241,7 +7539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G13" s="3">
         <v>9</v>
       </c>
@@ -7261,20 +7559,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A5:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="48" t="s">
         <v>58</v>
       </c>
@@ -7291,7 +7589,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="50">
         <v>210.5</v>
       </c>
@@ -7308,7 +7606,7 @@
         <v>188.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="50">
         <v>198.1</v>
       </c>
@@ -7325,7 +7623,7 @@
         <v>177.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="50">
         <v>145.30000000000001</v>
       </c>
@@ -7342,7 +7640,7 @@
         <v>176.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="50">
         <v>185.5</v>
       </c>
@@ -7359,7 +7657,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="50">
         <v>189.1</v>
       </c>
@@ -7376,7 +7674,7 @@
         <v>174.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="50">
         <v>135.9</v>
       </c>
@@ -7393,7 +7691,7 @@
         <v>181.7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="50">
         <v>180</v>
       </c>
@@ -7410,7 +7708,7 @@
         <v>176.2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="50">
         <v>149.4</v>
       </c>
@@ -7427,7 +7725,7 @@
         <v>177.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="50">
         <v>176.4</v>
       </c>
@@ -7444,7 +7742,7 @@
         <v>189.1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="50">
         <v>229</v>
       </c>
@@ -7461,7 +7759,7 @@
         <v>187.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -7489,16 +7787,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>